<commit_message>
Added download all feature
</commit_message>
<xml_diff>
--- a/static/TEMPLATE.xlsx
+++ b/static/TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\python\servers\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6205947-1E0A-4511-8C88-59D515DEC66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3302723-29C4-4CAC-BED8-39F11A84C634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BD1C55C-2772-4CE7-A10C-F71EC8289D89}"/>
   </bookViews>
@@ -171,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -267,14 +267,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -286,6 +304,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -310,51 +367,23 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1EC6FE-8DEF-454F-B437-D6BAA40647D3}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,368 +715,347 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="20" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="23" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="18" t="s">
+      <c r="L1" s="16"/>
+      <c r="M1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="1"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="34"/>
     </row>
-    <row r="2" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="1"/>
+    <row r="2" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="34"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="27" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="2"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="35"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="32">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="10">
         <v>6</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="10">
         <v>7</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="10">
         <v>8</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="10">
         <v>9</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="10">
         <v>10</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="10">
         <v>11</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="10">
         <v>12</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="10">
         <v>13</v>
       </c>
-      <c r="L4" s="32">
+      <c r="L4" s="10">
         <v>14</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="10">
         <v>15</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N4" s="10">
         <v>16</v>
       </c>
-      <c r="O4" s="32">
+      <c r="O4" s="10">
         <v>17</v>
       </c>
-      <c r="P4" s="32">
+    </row>
+    <row r="5" spans="1:16" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24">
+        <v>7620</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="8">
+        <v>67</v>
+      </c>
+      <c r="E5" s="8">
+        <v>76</v>
+      </c>
+      <c r="F5" s="8">
+        <v>67</v>
+      </c>
+      <c r="G5" s="8">
+        <v>76</v>
+      </c>
+      <c r="H5" s="8">
+        <v>67</v>
+      </c>
+      <c r="I5" s="8">
+        <v>76</v>
+      </c>
+      <c r="J5" s="8">
+        <v>67</v>
+      </c>
+      <c r="K5" s="8">
+        <v>76</v>
+      </c>
+      <c r="L5" s="8">
+        <v>67</v>
+      </c>
+      <c r="M5" s="8">
+        <v>76</v>
+      </c>
+      <c r="N5" s="8">
+        <v>67</v>
+      </c>
+      <c r="O5" s="8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="23">
+        <v>42</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="8">
+        <v>67</v>
+      </c>
+      <c r="E6" s="8">
+        <v>76</v>
+      </c>
+      <c r="F6" s="8">
+        <v>67</v>
+      </c>
+      <c r="G6" s="8">
+        <v>76</v>
+      </c>
+      <c r="H6" s="8">
+        <v>67</v>
+      </c>
+      <c r="I6" s="8">
+        <v>76</v>
+      </c>
+      <c r="J6" s="8">
+        <v>67</v>
+      </c>
+      <c r="K6" s="8">
+        <v>76</v>
+      </c>
+      <c r="L6" s="8">
+        <v>67</v>
+      </c>
+      <c r="M6" s="8">
+        <v>76</v>
+      </c>
+      <c r="N6" s="8">
+        <v>67</v>
+      </c>
+      <c r="O6" s="8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="10">
         <v>18</v>
       </c>
+      <c r="E7" s="10">
+        <v>19</v>
+      </c>
+      <c r="F7" s="10">
+        <v>20</v>
+      </c>
+      <c r="G7" s="10">
+        <v>21</v>
+      </c>
+      <c r="H7" s="10">
+        <v>22</v>
+      </c>
+      <c r="I7" s="10">
+        <v>23</v>
+      </c>
+      <c r="J7" s="10">
+        <v>24</v>
+      </c>
+      <c r="K7" s="10">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10">
+        <v>2</v>
+      </c>
+      <c r="M7" s="10">
+        <v>3</v>
+      </c>
+      <c r="N7" s="10">
+        <v>4</v>
+      </c>
+      <c r="O7" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="8" spans="1:16" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13">
-        <v>7620</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="30">
-        <v>67</v>
-      </c>
-      <c r="E5" s="30">
-        <v>76</v>
-      </c>
-      <c r="F5" s="30">
-        <v>67</v>
-      </c>
-      <c r="G5" s="30">
-        <v>76</v>
-      </c>
-      <c r="H5" s="30">
-        <v>67</v>
-      </c>
-      <c r="I5" s="30">
-        <v>76</v>
-      </c>
-      <c r="J5" s="30">
-        <v>67</v>
-      </c>
-      <c r="K5" s="30">
-        <v>76</v>
-      </c>
-      <c r="L5" s="30">
-        <v>67</v>
-      </c>
-      <c r="M5" s="30">
-        <v>76</v>
-      </c>
-      <c r="N5" s="30">
-        <v>67</v>
-      </c>
-      <c r="O5" s="30">
-        <v>76</v>
-      </c>
-      <c r="P5" s="30">
-        <v>67</v>
+      <c r="B8" s="22">
+        <v>6870</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="9">
+        <v>67</v>
+      </c>
+      <c r="E8" s="9">
+        <v>76</v>
+      </c>
+      <c r="F8" s="9">
+        <v>67</v>
+      </c>
+      <c r="G8" s="9">
+        <v>76</v>
+      </c>
+      <c r="H8" s="9">
+        <v>67</v>
+      </c>
+      <c r="I8" s="9">
+        <v>76</v>
+      </c>
+      <c r="J8" s="9">
+        <v>67</v>
+      </c>
+      <c r="K8" s="9">
+        <v>76</v>
+      </c>
+      <c r="L8" s="9">
+        <v>67</v>
+      </c>
+      <c r="M8" s="9">
+        <v>76</v>
+      </c>
+      <c r="N8" s="9">
+        <v>67</v>
+      </c>
+      <c r="O8" s="9">
+        <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="9" spans="1:16" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
-        <v>42</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="30">
-        <v>67</v>
-      </c>
-      <c r="E6" s="30">
-        <v>76</v>
-      </c>
-      <c r="F6" s="30">
-        <v>67</v>
-      </c>
-      <c r="G6" s="30">
-        <v>76</v>
-      </c>
-      <c r="H6" s="30">
-        <v>67</v>
-      </c>
-      <c r="I6" s="30">
-        <v>76</v>
-      </c>
-      <c r="J6" s="30">
-        <v>67</v>
-      </c>
-      <c r="K6" s="30">
-        <v>76</v>
-      </c>
-      <c r="L6" s="30">
-        <v>67</v>
-      </c>
-      <c r="M6" s="30">
-        <v>76</v>
-      </c>
-      <c r="N6" s="30">
-        <v>67</v>
-      </c>
-      <c r="O6" s="30">
-        <v>76</v>
-      </c>
-      <c r="P6" s="30">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="32">
-        <v>18</v>
-      </c>
-      <c r="E7" s="32">
-        <v>19</v>
-      </c>
-      <c r="F7" s="32">
-        <v>20</v>
-      </c>
-      <c r="G7" s="32">
-        <v>21</v>
-      </c>
-      <c r="H7" s="32">
-        <v>22</v>
-      </c>
-      <c r="I7" s="32">
-        <v>23</v>
-      </c>
-      <c r="J7" s="32">
-        <v>24</v>
-      </c>
-      <c r="K7" s="32">
-        <v>1</v>
-      </c>
-      <c r="L7" s="32">
-        <v>2</v>
-      </c>
-      <c r="M7" s="32">
-        <v>3</v>
-      </c>
-      <c r="N7" s="32">
-        <v>4</v>
-      </c>
-      <c r="O7" s="32">
-        <v>5</v>
-      </c>
-      <c r="P7" s="32">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="11">
-        <v>6870</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="31">
-        <v>67</v>
-      </c>
-      <c r="E8" s="31">
-        <v>76</v>
-      </c>
-      <c r="F8" s="31">
-        <v>67</v>
-      </c>
-      <c r="G8" s="31">
-        <v>76</v>
-      </c>
-      <c r="H8" s="31">
-        <v>67</v>
-      </c>
-      <c r="I8" s="31">
-        <v>76</v>
-      </c>
-      <c r="J8" s="31">
-        <v>67</v>
-      </c>
-      <c r="K8" s="31">
-        <v>76</v>
-      </c>
-      <c r="L8" s="31">
-        <v>67</v>
-      </c>
-      <c r="M8" s="31">
-        <v>76</v>
-      </c>
-      <c r="N8" s="31">
-        <v>67</v>
-      </c>
-      <c r="O8" s="31">
-        <v>76</v>
-      </c>
-      <c r="P8" s="31">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="10">
+      <c r="B9" s="21">
         <v>32</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="31">
-        <v>67</v>
-      </c>
-      <c r="E9" s="31">
-        <v>76</v>
-      </c>
-      <c r="F9" s="31">
-        <v>67</v>
-      </c>
-      <c r="G9" s="31">
-        <v>76</v>
-      </c>
-      <c r="H9" s="31">
-        <v>67</v>
-      </c>
-      <c r="I9" s="31">
-        <v>76</v>
-      </c>
-      <c r="J9" s="31">
-        <v>67</v>
-      </c>
-      <c r="K9" s="31">
-        <v>76</v>
-      </c>
-      <c r="L9" s="31">
-        <v>67</v>
-      </c>
-      <c r="M9" s="31">
-        <v>76</v>
-      </c>
-      <c r="N9" s="31">
-        <v>67</v>
-      </c>
-      <c r="O9" s="31">
-        <v>76</v>
-      </c>
-      <c r="P9" s="31">
-        <v>67</v>
+      <c r="C9" s="21"/>
+      <c r="D9" s="9">
+        <v>67</v>
+      </c>
+      <c r="E9" s="9">
+        <v>76</v>
+      </c>
+      <c r="F9" s="9">
+        <v>67</v>
+      </c>
+      <c r="G9" s="9">
+        <v>76</v>
+      </c>
+      <c r="H9" s="9">
+        <v>67</v>
+      </c>
+      <c r="I9" s="9">
+        <v>76</v>
+      </c>
+      <c r="J9" s="9">
+        <v>67</v>
+      </c>
+      <c r="K9" s="9">
+        <v>76</v>
+      </c>
+      <c r="L9" s="9">
+        <v>67</v>
+      </c>
+      <c r="M9" s="9">
+        <v>76</v>
+      </c>
+      <c r="N9" s="9">
+        <v>67</v>
+      </c>
+      <c r="O9" s="9">
+        <v>76</v>
       </c>
     </row>
     <row r="19" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="M1:P2"/>
-    <mergeCell ref="G1:J2"/>
-    <mergeCell ref="K1:L2"/>
-    <mergeCell ref="D3:P3"/>
-    <mergeCell ref="A1:F2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B3:C4"/>
+    <mergeCell ref="G1:J2"/>
+    <mergeCell ref="K1:L2"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="D3:O3"/>
+    <mergeCell ref="M1:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>